<commit_message>
Cleaning up some stuff
</commit_message>
<xml_diff>
--- a/results/Makefile-Graph.xlsx
+++ b/results/Makefile-Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lenovo\Documents\code\SCons-Make-Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A3582-5468-4C09-93CB-2CE657C89088}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4410BFF-72F6-43BB-98EE-62EFC6F842AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="184">
   <si>
     <t>Repository name</t>
   </si>
@@ -571,6 +571,15 @@
   </si>
   <si>
     <t>Sum Repo Size (MB)</t>
+  </si>
+  <si>
+    <t>Sum Lines added</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sum Lines removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sum No. Commits</t>
   </si>
 </sst>
 </file>
@@ -2163,7 +2172,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3469,7 +3477,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -8126,8 +8133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11825,6 +11832,15 @@
       <c r="E155" t="s">
         <v>176</v>
       </c>
+      <c r="F155" t="s">
+        <v>181</v>
+      </c>
+      <c r="G155" t="s">
+        <v>182</v>
+      </c>
+      <c r="H155" t="s">
+        <v>183</v>
+      </c>
       <c r="J155" t="s">
         <v>179</v>
       </c>
@@ -11848,6 +11864,15 @@
       <c r="E156">
         <v>1421589183</v>
       </c>
+      <c r="F156">
+        <v>180</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156">
+        <v>2</v>
+      </c>
       <c r="J156">
         <f>D156/1024</f>
         <v>6.7490234375</v>
@@ -11873,6 +11898,15 @@
       <c r="E157">
         <v>1405076776</v>
       </c>
+      <c r="F157">
+        <v>16</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157">
+        <v>2</v>
+      </c>
       <c r="J157">
         <f t="shared" ref="J157:J220" si="3">D157/1024</f>
         <v>0.486328125</v>
@@ -11898,6 +11932,15 @@
       <c r="E158">
         <v>1405882272</v>
       </c>
+      <c r="F158">
+        <v>14</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
       <c r="J158">
         <f t="shared" si="3"/>
         <v>0.486328125</v>
@@ -11923,6 +11966,15 @@
       <c r="E159">
         <v>1418210724</v>
       </c>
+      <c r="F159">
+        <v>19</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>2</v>
+      </c>
       <c r="J159">
         <f t="shared" si="3"/>
         <v>0.2626953125</v>
@@ -11948,6 +12000,15 @@
       <c r="E160">
         <v>1327052706</v>
       </c>
+      <c r="F160">
+        <v>22</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>2</v>
+      </c>
       <c r="J160">
         <f t="shared" si="3"/>
         <v>0.75</v>
@@ -11973,6 +12034,15 @@
       <c r="E161">
         <v>1395578883</v>
       </c>
+      <c r="F161">
+        <v>791</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>41</v>
+      </c>
       <c r="J161">
         <f t="shared" si="3"/>
         <v>18.5078125</v>
@@ -11998,6 +12068,15 @@
       <c r="E162">
         <v>1436104818</v>
       </c>
+      <c r="F162">
+        <v>13</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+      <c r="H162">
+        <v>4</v>
+      </c>
       <c r="J162">
         <f t="shared" si="3"/>
         <v>0.373046875</v>
@@ -12023,6 +12102,15 @@
       <c r="E163">
         <v>1267250657</v>
       </c>
+      <c r="F163">
+        <v>332</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="H163">
+        <v>1</v>
+      </c>
       <c r="J163">
         <f t="shared" si="3"/>
         <v>10.2216796875</v>
@@ -12048,6 +12136,15 @@
       <c r="E164">
         <v>1427110514</v>
       </c>
+      <c r="F164">
+        <v>91</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>6</v>
+      </c>
       <c r="J164">
         <f t="shared" si="3"/>
         <v>1.845703125</v>
@@ -12073,6 +12170,15 @@
       <c r="E165">
         <v>1420017859</v>
       </c>
+      <c r="F165">
+        <v>43</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165">
+        <v>1</v>
+      </c>
       <c r="J165">
         <f t="shared" si="3"/>
         <v>1.072265625</v>
@@ -12098,6 +12204,15 @@
       <c r="E166">
         <v>1403962359</v>
       </c>
+      <c r="F166">
+        <v>799</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166">
+        <v>41</v>
+      </c>
       <c r="J166">
         <f t="shared" si="3"/>
         <v>19.2724609375</v>
@@ -12123,6 +12238,15 @@
       <c r="E167">
         <v>1390806411</v>
       </c>
+      <c r="F167">
+        <v>333</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
       <c r="J167">
         <f t="shared" si="3"/>
         <v>20.1142578125</v>
@@ -12148,6 +12272,15 @@
       <c r="E168">
         <v>1434278868</v>
       </c>
+      <c r="F168">
+        <v>10</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="H168">
+        <v>1</v>
+      </c>
       <c r="J168">
         <f t="shared" si="3"/>
         <v>0.271484375</v>
@@ -12173,6 +12306,15 @@
       <c r="E169">
         <v>1190025051</v>
       </c>
+      <c r="F169">
+        <v>299</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
+      <c r="H169">
+        <v>85</v>
+      </c>
       <c r="J169">
         <f t="shared" si="3"/>
         <v>4.3154296875</v>
@@ -12198,6 +12340,15 @@
       <c r="E170">
         <v>1405272124</v>
       </c>
+      <c r="F170">
+        <v>420</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+      <c r="H170">
+        <v>24</v>
+      </c>
       <c r="J170">
         <f t="shared" si="3"/>
         <v>9.69921875</v>
@@ -12223,6 +12374,15 @@
       <c r="E171">
         <v>1418403333</v>
       </c>
+      <c r="F171">
+        <v>36</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+      <c r="H171">
+        <v>6</v>
+      </c>
       <c r="J171">
         <f t="shared" si="3"/>
         <v>0.3388671875</v>
@@ -12248,6 +12408,15 @@
       <c r="E172">
         <v>1473154296</v>
       </c>
+      <c r="F172">
+        <v>11</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172">
+        <v>3</v>
+      </c>
       <c r="J172">
         <f t="shared" si="3"/>
         <v>8.30078125E-2</v>
@@ -12273,6 +12442,15 @@
       <c r="E173">
         <v>1476084819</v>
       </c>
+      <c r="F173">
+        <v>110</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>3</v>
+      </c>
       <c r="J173">
         <f t="shared" si="3"/>
         <v>2.3525390625</v>
@@ -12298,6 +12476,15 @@
       <c r="E174">
         <v>1380368846</v>
       </c>
+      <c r="F174">
+        <v>189</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
+      <c r="H174">
+        <v>29</v>
+      </c>
       <c r="J174">
         <f t="shared" si="3"/>
         <v>2.38671875</v>
@@ -12323,6 +12510,15 @@
       <c r="E175">
         <v>1423166240</v>
       </c>
+      <c r="F175">
+        <v>32</v>
+      </c>
+      <c r="G175">
+        <v>0</v>
+      </c>
+      <c r="H175">
+        <v>2</v>
+      </c>
       <c r="J175">
         <f t="shared" si="3"/>
         <v>0.57421875</v>
@@ -12348,6 +12544,15 @@
       <c r="E176">
         <v>1443097293</v>
       </c>
+      <c r="F176">
+        <v>83</v>
+      </c>
+      <c r="G176">
+        <v>0</v>
+      </c>
+      <c r="H176">
+        <v>3</v>
+      </c>
       <c r="J176">
         <f t="shared" si="3"/>
         <v>2.1298828125</v>
@@ -12373,6 +12578,15 @@
       <c r="E177">
         <v>1418383720</v>
       </c>
+      <c r="F177">
+        <v>101</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
+      <c r="H177">
+        <v>8</v>
+      </c>
       <c r="J177">
         <f t="shared" si="3"/>
         <v>1.9775390625</v>
@@ -12398,6 +12612,15 @@
       <c r="E178">
         <v>1402317137</v>
       </c>
+      <c r="F178">
+        <v>15</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
+      <c r="H178">
+        <v>10</v>
+      </c>
       <c r="J178">
         <f t="shared" si="3"/>
         <v>0.2646484375</v>
@@ -12423,6 +12646,15 @@
       <c r="E179">
         <v>1301412885</v>
       </c>
+      <c r="F179">
+        <v>484</v>
+      </c>
+      <c r="G179">
+        <v>0</v>
+      </c>
+      <c r="H179">
+        <v>11</v>
+      </c>
       <c r="J179">
         <f t="shared" si="3"/>
         <v>7.2685546875</v>
@@ -12448,6 +12680,15 @@
       <c r="E180">
         <v>1250523600</v>
       </c>
+      <c r="F180">
+        <v>237</v>
+      </c>
+      <c r="G180">
+        <v>0</v>
+      </c>
+      <c r="H180">
+        <v>1</v>
+      </c>
       <c r="J180">
         <f t="shared" si="3"/>
         <v>6.6396484375</v>
@@ -12473,6 +12714,15 @@
       <c r="E181">
         <v>1297743189</v>
       </c>
+      <c r="F181">
+        <v>376</v>
+      </c>
+      <c r="G181">
+        <v>0</v>
+      </c>
+      <c r="H181">
+        <v>1</v>
+      </c>
       <c r="J181">
         <f t="shared" si="3"/>
         <v>11.0869140625</v>
@@ -12498,6 +12748,15 @@
       <c r="E182">
         <v>1520192648</v>
       </c>
+      <c r="F182">
+        <v>68</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182">
+        <v>1</v>
+      </c>
       <c r="J182">
         <f t="shared" si="3"/>
         <v>1.794921875</v>
@@ -12523,6 +12782,15 @@
       <c r="E183">
         <v>1470758876</v>
       </c>
+      <c r="F183">
+        <v>230</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>2</v>
+      </c>
       <c r="J183">
         <f t="shared" si="3"/>
         <v>8.7880859375</v>
@@ -12548,6 +12816,15 @@
       <c r="E184">
         <v>1444797501</v>
       </c>
+      <c r="F184">
+        <v>124</v>
+      </c>
+      <c r="G184">
+        <v>0</v>
+      </c>
+      <c r="H184">
+        <v>20</v>
+      </c>
       <c r="J184">
         <f t="shared" si="3"/>
         <v>1.966796875</v>
@@ -12573,6 +12850,15 @@
       <c r="E185">
         <v>1333000040</v>
       </c>
+      <c r="F185">
+        <v>66</v>
+      </c>
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="H185">
+        <v>7</v>
+      </c>
       <c r="J185">
         <f t="shared" si="3"/>
         <v>0.7333984375</v>
@@ -12598,6 +12884,15 @@
       <c r="E186">
         <v>1442188143</v>
       </c>
+      <c r="F186">
+        <v>95</v>
+      </c>
+      <c r="G186">
+        <v>0</v>
+      </c>
+      <c r="H186">
+        <v>12</v>
+      </c>
       <c r="J186">
         <f t="shared" si="3"/>
         <v>1.306640625</v>
@@ -12623,6 +12918,15 @@
       <c r="E187">
         <v>1429446513</v>
       </c>
+      <c r="F187">
+        <v>16</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <v>1</v>
+      </c>
       <c r="J187">
         <f t="shared" si="3"/>
         <v>0.271484375</v>
@@ -12648,6 +12952,15 @@
       <c r="E188">
         <v>1483443113</v>
       </c>
+      <c r="F188">
+        <v>153</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188">
+        <v>7</v>
+      </c>
       <c r="J188">
         <f t="shared" si="3"/>
         <v>2.8984375</v>
@@ -12673,6 +12986,15 @@
       <c r="E189">
         <v>1458431281</v>
       </c>
+      <c r="F189">
+        <v>211</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
+      <c r="H189">
+        <v>4</v>
+      </c>
       <c r="J189">
         <f t="shared" si="3"/>
         <v>4.6806640625</v>
@@ -12698,6 +13020,15 @@
       <c r="E190">
         <v>1507299290</v>
       </c>
+      <c r="F190">
+        <v>6</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
+      <c r="H190">
+        <v>1</v>
+      </c>
       <c r="J190">
         <f t="shared" si="3"/>
         <v>0.1669921875</v>
@@ -12723,6 +13054,15 @@
       <c r="E191">
         <v>1379515274</v>
       </c>
+      <c r="F191">
+        <v>121</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>7</v>
+      </c>
       <c r="J191">
         <f t="shared" si="3"/>
         <v>2.3203125</v>
@@ -12748,6 +13088,15 @@
       <c r="E192">
         <v>1437170541</v>
       </c>
+      <c r="F192">
+        <v>198</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>3</v>
+      </c>
       <c r="J192">
         <f t="shared" si="3"/>
         <v>6.201171875</v>
@@ -12773,6 +13122,15 @@
       <c r="E193">
         <v>1291155194</v>
       </c>
+      <c r="F193">
+        <v>37</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>3</v>
+      </c>
       <c r="J193">
         <f t="shared" si="3"/>
         <v>1.02734375</v>
@@ -12798,6 +13156,15 @@
       <c r="E194">
         <v>1410449124</v>
       </c>
+      <c r="F194">
+        <v>82</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194">
+        <v>11</v>
+      </c>
       <c r="J194">
         <f t="shared" si="3"/>
         <v>1.966796875</v>
@@ -12823,6 +13190,15 @@
       <c r="E195">
         <v>1493225915</v>
       </c>
+      <c r="F195">
+        <v>96</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195">
+        <v>9</v>
+      </c>
       <c r="J195">
         <f t="shared" si="3"/>
         <v>0.7763671875</v>
@@ -12848,6 +13224,15 @@
       <c r="E196">
         <v>1439358993</v>
       </c>
+      <c r="F196">
+        <v>55</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
+      <c r="H196">
+        <v>3</v>
+      </c>
       <c r="J196">
         <f t="shared" si="3"/>
         <v>1.349609375</v>
@@ -12873,6 +13258,15 @@
       <c r="E197">
         <v>1418699110</v>
       </c>
+      <c r="F197">
+        <v>16</v>
+      </c>
+      <c r="G197">
+        <v>0</v>
+      </c>
+      <c r="H197">
+        <v>1</v>
+      </c>
       <c r="J197">
         <f t="shared" si="3"/>
         <v>0.3271484375</v>
@@ -12898,6 +13292,15 @@
       <c r="E198">
         <v>1413354345</v>
       </c>
+      <c r="F198">
+        <v>5</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>2</v>
+      </c>
       <c r="J198">
         <f t="shared" si="3"/>
         <v>0.1806640625</v>
@@ -12923,6 +13326,15 @@
       <c r="E199">
         <v>1296524633</v>
       </c>
+      <c r="F199">
+        <v>1812</v>
+      </c>
+      <c r="G199">
+        <v>0</v>
+      </c>
+      <c r="H199">
+        <v>31</v>
+      </c>
       <c r="J199">
         <f t="shared" si="3"/>
         <v>46.013671875</v>
@@ -12948,6 +13360,15 @@
       <c r="E200">
         <v>1413540483</v>
       </c>
+      <c r="F200">
+        <v>19</v>
+      </c>
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>2</v>
+      </c>
       <c r="J200">
         <f t="shared" si="3"/>
         <v>0.3662109375</v>
@@ -12973,6 +13394,15 @@
       <c r="E201">
         <v>1449453411</v>
       </c>
+      <c r="F201">
+        <v>106</v>
+      </c>
+      <c r="G201">
+        <v>0</v>
+      </c>
+      <c r="H201">
+        <v>7</v>
+      </c>
       <c r="J201">
         <f t="shared" si="3"/>
         <v>2.8857421875</v>
@@ -12998,6 +13428,15 @@
       <c r="E202">
         <v>1392804583</v>
       </c>
+      <c r="F202">
+        <v>22</v>
+      </c>
+      <c r="G202">
+        <v>0</v>
+      </c>
+      <c r="H202">
+        <v>2</v>
+      </c>
       <c r="J202">
         <f t="shared" si="3"/>
         <v>0.3857421875</v>
@@ -13023,6 +13462,15 @@
       <c r="E203">
         <v>1361612142</v>
       </c>
+      <c r="F203">
+        <v>4</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+      <c r="H203">
+        <v>2</v>
+      </c>
       <c r="J203">
         <f t="shared" si="3"/>
         <v>0.208984375</v>
@@ -13048,6 +13496,15 @@
       <c r="E204">
         <v>1237377773</v>
       </c>
+      <c r="F204">
+        <v>70</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204">
+        <v>24</v>
+      </c>
       <c r="J204">
         <f t="shared" si="3"/>
         <v>0.326171875</v>
@@ -13073,6 +13530,15 @@
       <c r="E205">
         <v>1380807159</v>
       </c>
+      <c r="F205">
+        <v>789</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205">
+        <v>4</v>
+      </c>
       <c r="J205">
         <f t="shared" si="3"/>
         <v>26.4248046875</v>
@@ -13098,6 +13564,15 @@
       <c r="E206">
         <v>1281603913</v>
       </c>
+      <c r="F206">
+        <v>66</v>
+      </c>
+      <c r="G206">
+        <v>0</v>
+      </c>
+      <c r="H206">
+        <v>17</v>
+      </c>
       <c r="J206">
         <f t="shared" si="3"/>
         <v>0.4052734375</v>
@@ -13123,6 +13598,15 @@
       <c r="E207">
         <v>1391041947</v>
       </c>
+      <c r="F207">
+        <v>145</v>
+      </c>
+      <c r="G207">
+        <v>0</v>
+      </c>
+      <c r="H207">
+        <v>3</v>
+      </c>
       <c r="J207">
         <f t="shared" si="3"/>
         <v>4.298828125</v>
@@ -13148,6 +13632,15 @@
       <c r="E208">
         <v>1443196232</v>
       </c>
+      <c r="F208">
+        <v>105</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
+      <c r="H208">
+        <v>8</v>
+      </c>
       <c r="J208">
         <f t="shared" si="3"/>
         <v>0.29296875</v>
@@ -13173,6 +13666,15 @@
       <c r="E209">
         <v>1332362735</v>
       </c>
+      <c r="F209">
+        <v>32</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
+      <c r="H209">
+        <v>4</v>
+      </c>
       <c r="J209">
         <f t="shared" si="3"/>
         <v>0.47265625</v>
@@ -13198,6 +13700,15 @@
       <c r="E210">
         <v>1367829269</v>
       </c>
+      <c r="F210">
+        <v>59</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
+      <c r="H210">
+        <v>6</v>
+      </c>
       <c r="J210">
         <f t="shared" si="3"/>
         <v>0.7275390625</v>
@@ -13223,6 +13734,15 @@
       <c r="E211">
         <v>1387389240</v>
       </c>
+      <c r="F211">
+        <v>290</v>
+      </c>
+      <c r="G211">
+        <v>0</v>
+      </c>
+      <c r="H211">
+        <v>3</v>
+      </c>
       <c r="J211">
         <f t="shared" si="3"/>
         <v>11.0888671875</v>
@@ -13248,6 +13768,15 @@
       <c r="E212">
         <v>1435627274</v>
       </c>
+      <c r="F212">
+        <v>40</v>
+      </c>
+      <c r="G212">
+        <v>0</v>
+      </c>
+      <c r="H212">
+        <v>1</v>
+      </c>
       <c r="J212">
         <f t="shared" si="3"/>
         <v>1.5458984375</v>
@@ -13273,6 +13802,15 @@
       <c r="E213">
         <v>1458815593</v>
       </c>
+      <c r="F213">
+        <v>20</v>
+      </c>
+      <c r="G213">
+        <v>0</v>
+      </c>
+      <c r="H213">
+        <v>1</v>
+      </c>
       <c r="J213">
         <f t="shared" si="3"/>
         <v>0.54296875</v>
@@ -13298,6 +13836,15 @@
       <c r="E214">
         <v>1430682030</v>
       </c>
+      <c r="F214">
+        <v>17</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214">
+        <v>1</v>
+      </c>
       <c r="J214">
         <f t="shared" si="3"/>
         <v>0.6396484375</v>
@@ -13323,6 +13870,15 @@
       <c r="E215">
         <v>1454092816</v>
       </c>
+      <c r="F215">
+        <v>38</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+      <c r="H215">
+        <v>1</v>
+      </c>
       <c r="J215">
         <f t="shared" si="3"/>
         <v>0.9267578125</v>
@@ -13348,6 +13904,15 @@
       <c r="E216">
         <v>1383378294</v>
       </c>
+      <c r="F216">
+        <v>51</v>
+      </c>
+      <c r="G216">
+        <v>0</v>
+      </c>
+      <c r="H216">
+        <v>11</v>
+      </c>
       <c r="J216">
         <f t="shared" si="3"/>
         <v>0.9873046875</v>
@@ -13373,6 +13938,15 @@
       <c r="E217">
         <v>1485208921</v>
       </c>
+      <c r="F217">
+        <v>538</v>
+      </c>
+      <c r="G217">
+        <v>0</v>
+      </c>
+      <c r="H217">
+        <v>17</v>
+      </c>
       <c r="J217">
         <f t="shared" si="3"/>
         <v>18.4443359375</v>
@@ -13398,6 +13972,15 @@
       <c r="E218">
         <v>1490046451</v>
       </c>
+      <c r="F218">
+        <v>10</v>
+      </c>
+      <c r="G218">
+        <v>0</v>
+      </c>
+      <c r="H218">
+        <v>1</v>
+      </c>
       <c r="J218">
         <f t="shared" si="3"/>
         <v>0.2392578125</v>
@@ -13423,6 +14006,15 @@
       <c r="E219">
         <v>1424354280</v>
       </c>
+      <c r="F219">
+        <v>14</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
+      <c r="H219">
+        <v>7</v>
+      </c>
       <c r="J219">
         <f t="shared" si="3"/>
         <v>7.51953125E-2</v>
@@ -13448,6 +14040,15 @@
       <c r="E220">
         <v>1280070525</v>
       </c>
+      <c r="F220">
+        <v>107</v>
+      </c>
+      <c r="G220">
+        <v>0</v>
+      </c>
+      <c r="H220">
+        <v>12</v>
+      </c>
       <c r="J220">
         <f t="shared" si="3"/>
         <v>1.9716796875</v>
@@ -13473,6 +14074,15 @@
       <c r="E221">
         <v>1428371019</v>
       </c>
+      <c r="F221">
+        <v>32</v>
+      </c>
+      <c r="G221">
+        <v>0</v>
+      </c>
+      <c r="H221">
+        <v>2</v>
+      </c>
       <c r="J221">
         <f t="shared" ref="J221:J226" si="5">D221/1024</f>
         <v>1.306640625</v>
@@ -13498,6 +14108,15 @@
       <c r="E222">
         <v>1384314206</v>
       </c>
+      <c r="F222">
+        <v>81</v>
+      </c>
+      <c r="G222">
+        <v>0</v>
+      </c>
+      <c r="H222">
+        <v>4</v>
+      </c>
       <c r="J222">
         <f t="shared" si="5"/>
         <v>2.197265625</v>
@@ -13523,6 +14142,15 @@
       <c r="E223">
         <v>1312602157</v>
       </c>
+      <c r="F223">
+        <v>313</v>
+      </c>
+      <c r="G223">
+        <v>0</v>
+      </c>
+      <c r="H223">
+        <v>3</v>
+      </c>
       <c r="J223">
         <f t="shared" si="5"/>
         <v>10.0029296875</v>
@@ -13548,6 +14176,15 @@
       <c r="E224">
         <v>1403308739</v>
       </c>
+      <c r="F224">
+        <v>501</v>
+      </c>
+      <c r="G224">
+        <v>0</v>
+      </c>
+      <c r="H224">
+        <v>36</v>
+      </c>
       <c r="J224">
         <f t="shared" si="5"/>
         <v>0.232421875</v>
@@ -13573,6 +14210,15 @@
       <c r="E225">
         <v>1415947757</v>
       </c>
+      <c r="F225">
+        <v>95</v>
+      </c>
+      <c r="G225">
+        <v>0</v>
+      </c>
+      <c r="H225">
+        <v>5</v>
+      </c>
       <c r="J225">
         <f t="shared" si="5"/>
         <v>1.0087890625</v>
@@ -13597,6 +14243,15 @@
       </c>
       <c r="E226">
         <v>1453923051</v>
+      </c>
+      <c r="F226">
+        <v>16</v>
+      </c>
+      <c r="G226">
+        <v>0</v>
+      </c>
+      <c r="H226">
+        <v>10</v>
       </c>
       <c r="J226">
         <f t="shared" si="5"/>

</xml_diff>

<commit_message>
Finally got some kind of useful graphs
</commit_message>
<xml_diff>
--- a/results/Makefile-Graph.xlsx
+++ b/results/Makefile-Graph.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lenovo\Documents\code\SCons-Make-Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4410BFF-72F6-43BB-98EE-62EFC6F842AC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2B5AE6-3EF8-4624-8BE8-683003A2A47B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Makefile" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Makefile!$G$155</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Makefile!$G$156:$G$226</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Makefile!$G$155</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Makefile!$G$156:$G$226</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -5472,6 +5478,131 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Repository with lines deleted</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Repository with lines deleted</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{9FC97550-66BC-407A-9F1A-FB9F17ED68E5}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v> Sum Lines removed</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binSize val="15"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>Lines deleted</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>Lines deleted</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title>
+          <cx:tx>
+            <cx:txData>
+              <cx:v>No. Repos</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:txPr>
+            <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                </a:rPr>
+                <a:t>No. Repos</a:t>
+              </a:r>
+            </a:p>
+          </cx:txPr>
+        </cx:title>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5593,6 +5724,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7685,6 +7856,514 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7829,6 +8508,84 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276679</xdr:colOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>11792</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>979714</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>45356</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8294A29-B25E-48A2-80B7-54B76637DEE6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="276679" y="41377506"/>
+              <a:ext cx="7071178" cy="3299279"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8133,8 +8890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F156" sqref="F156"/>
+    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K239" sqref="K239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11868,7 +12625,7 @@
         <v>180</v>
       </c>
       <c r="G156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H156">
         <v>2</v>
@@ -11902,7 +12659,7 @@
         <v>16</v>
       </c>
       <c r="G157">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H157">
         <v>2</v>
@@ -11970,7 +12727,7 @@
         <v>19</v>
       </c>
       <c r="G159">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H159">
         <v>2</v>
@@ -12038,7 +12795,7 @@
         <v>791</v>
       </c>
       <c r="G161">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="H161">
         <v>41</v>
@@ -12072,7 +12829,7 @@
         <v>13</v>
       </c>
       <c r="G162">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H162">
         <v>4</v>
@@ -12140,7 +12897,7 @@
         <v>91</v>
       </c>
       <c r="G164">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H164">
         <v>6</v>
@@ -12208,7 +12965,7 @@
         <v>799</v>
       </c>
       <c r="G166">
-        <v>0</v>
+        <v>318</v>
       </c>
       <c r="H166">
         <v>41</v>
@@ -12310,7 +13067,7 @@
         <v>299</v>
       </c>
       <c r="G169">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="H169">
         <v>85</v>
@@ -12344,7 +13101,7 @@
         <v>420</v>
       </c>
       <c r="G170">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="H170">
         <v>24</v>
@@ -12378,7 +13135,7 @@
         <v>36</v>
       </c>
       <c r="G171">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H171">
         <v>6</v>
@@ -12412,7 +13169,7 @@
         <v>11</v>
       </c>
       <c r="G172">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H172">
         <v>3</v>
@@ -12446,7 +13203,7 @@
         <v>110</v>
       </c>
       <c r="G173">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H173">
         <v>3</v>
@@ -12480,7 +13237,7 @@
         <v>189</v>
       </c>
       <c r="G174">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H174">
         <v>29</v>
@@ -12514,7 +13271,7 @@
         <v>32</v>
       </c>
       <c r="G175">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H175">
         <v>2</v>
@@ -12548,7 +13305,7 @@
         <v>83</v>
       </c>
       <c r="G176">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H176">
         <v>3</v>
@@ -12582,7 +13339,7 @@
         <v>101</v>
       </c>
       <c r="G177">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H177">
         <v>8</v>
@@ -12616,7 +13373,7 @@
         <v>15</v>
       </c>
       <c r="G178">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H178">
         <v>10</v>
@@ -12650,7 +13407,7 @@
         <v>484</v>
       </c>
       <c r="G179">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="H179">
         <v>11</v>
@@ -12786,7 +13543,7 @@
         <v>230</v>
       </c>
       <c r="G183">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H183">
         <v>2</v>
@@ -12820,7 +13577,7 @@
         <v>124</v>
       </c>
       <c r="G184">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H184">
         <v>20</v>
@@ -12854,7 +13611,7 @@
         <v>66</v>
       </c>
       <c r="G185">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H185">
         <v>7</v>
@@ -12888,7 +13645,7 @@
         <v>95</v>
       </c>
       <c r="G186">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H186">
         <v>12</v>
@@ -12956,7 +13713,7 @@
         <v>153</v>
       </c>
       <c r="G188">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H188">
         <v>7</v>
@@ -12990,7 +13747,7 @@
         <v>211</v>
       </c>
       <c r="G189">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H189">
         <v>4</v>
@@ -13058,7 +13815,7 @@
         <v>121</v>
       </c>
       <c r="G191">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H191">
         <v>7</v>
@@ -13092,7 +13849,7 @@
         <v>198</v>
       </c>
       <c r="G192">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H192">
         <v>3</v>
@@ -13160,7 +13917,7 @@
         <v>82</v>
       </c>
       <c r="G194">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H194">
         <v>11</v>
@@ -13194,7 +13951,7 @@
         <v>96</v>
       </c>
       <c r="G195">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="H195">
         <v>9</v>
@@ -13228,7 +13985,7 @@
         <v>55</v>
       </c>
       <c r="G196">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H196">
         <v>3</v>
@@ -13330,7 +14087,7 @@
         <v>1812</v>
       </c>
       <c r="G199">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H199">
         <v>31</v>
@@ -13364,7 +14121,7 @@
         <v>19</v>
       </c>
       <c r="G200">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H200">
         <v>2</v>
@@ -13398,7 +14155,7 @@
         <v>106</v>
       </c>
       <c r="G201">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H201">
         <v>7</v>
@@ -13432,7 +14189,7 @@
         <v>22</v>
       </c>
       <c r="G202">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H202">
         <v>2</v>
@@ -13500,7 +14257,7 @@
         <v>70</v>
       </c>
       <c r="G204">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="H204">
         <v>24</v>
@@ -13568,7 +14325,7 @@
         <v>66</v>
       </c>
       <c r="G206">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="H206">
         <v>17</v>
@@ -13602,7 +14359,7 @@
         <v>145</v>
       </c>
       <c r="G207">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H207">
         <v>3</v>
@@ -13636,7 +14393,7 @@
         <v>105</v>
       </c>
       <c r="G208">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="H208">
         <v>8</v>
@@ -13670,7 +14427,7 @@
         <v>32</v>
       </c>
       <c r="G209">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H209">
         <v>4</v>
@@ -13704,7 +14461,7 @@
         <v>59</v>
       </c>
       <c r="G210">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H210">
         <v>6</v>
@@ -13908,7 +14665,7 @@
         <v>51</v>
       </c>
       <c r="G216">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H216">
         <v>11</v>
@@ -13942,7 +14699,7 @@
         <v>538</v>
       </c>
       <c r="G217">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H217">
         <v>17</v>
@@ -14044,7 +14801,7 @@
         <v>107</v>
       </c>
       <c r="G220">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H220">
         <v>12</v>
@@ -14078,7 +14835,7 @@
         <v>32</v>
       </c>
       <c r="G221">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H221">
         <v>2</v>
@@ -14112,7 +14869,7 @@
         <v>81</v>
       </c>
       <c r="G222">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H222">
         <v>4</v>
@@ -14146,7 +14903,7 @@
         <v>313</v>
       </c>
       <c r="G223">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H223">
         <v>3</v>
@@ -14180,7 +14937,7 @@
         <v>501</v>
       </c>
       <c r="G224">
-        <v>0</v>
+        <v>492</v>
       </c>
       <c r="H224">
         <v>36</v>
@@ -14214,7 +14971,7 @@
         <v>95</v>
       </c>
       <c r="G225">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="H225">
         <v>5</v>
@@ -14248,7 +15005,7 @@
         <v>16</v>
       </c>
       <c r="G226">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H226">
         <v>10</v>

</xml_diff>

<commit_message>
Cleaned up and added averages and medians
</commit_message>
<xml_diff>
--- a/results/Makefile-Graph.xlsx
+++ b/results/Makefile-Graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Lenovo\Documents\code\SCons-Make-Research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2B5AE6-3EF8-4624-8BE8-683003A2A47B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DFABFD-3E33-4690-A93E-C16FD703C327}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,6 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Makefile!$G$155</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Makefile!$G$156:$G$226</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Makefile!$G$155</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Makefile!$G$156:$G$226</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="186">
   <si>
     <t>Repository name</t>
   </si>
@@ -586,6 +584,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Sum No. Commits</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Median</t>
   </si>
 </sst>
 </file>
@@ -5483,7 +5487,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5491,7 +5495,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Repository with lines deleted</cx:v>
+          <cx:v>No. Repository with lines deleted</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -5511,7 +5515,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Repository with lines deleted</a:t>
+            <a:t>No. Repository with lines deleted</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -5521,7 +5525,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{9FC97550-66BC-407A-9F1A-FB9F17ED68E5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v> Sum Lines removed</cx:v>
             </cx:txData>
           </cx:tx>
@@ -8513,15 +8517,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>276679</xdr:colOff>
-      <xdr:row>228</xdr:row>
-      <xdr:rowOff>11792</xdr:rowOff>
+      <xdr:colOff>213179</xdr:colOff>
+      <xdr:row>230</xdr:row>
+      <xdr:rowOff>2721</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>979714</xdr:colOff>
-      <xdr:row>246</xdr:row>
-      <xdr:rowOff>45356</xdr:rowOff>
+      <xdr:colOff>916214</xdr:colOff>
+      <xdr:row>248</xdr:row>
+      <xdr:rowOff>36285</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -8557,7 +8561,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="276679" y="41377506"/>
+              <a:off x="213179" y="41731292"/>
               <a:ext cx="7071178" cy="3299279"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -8888,10 +8892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K227"/>
+  <dimension ref="A1:K229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K239" sqref="K239"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H229" sqref="B229:H229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15027,8 +15031,51 @@
         <v>151</v>
       </c>
     </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>184</v>
+      </c>
+      <c r="B228">
+        <f>AVERAGE(B156:B226)</f>
+        <v>2.140845070422535</v>
+      </c>
+      <c r="F228">
+        <f t="shared" ref="F228:H228" si="7">AVERAGE(F156:F226)</f>
+        <v>169.3943661971831</v>
+      </c>
+      <c r="G228">
+        <f t="shared" si="7"/>
+        <v>33.478873239436616</v>
+      </c>
+      <c r="H228">
+        <f t="shared" si="7"/>
+        <v>8.591549295774648</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>185</v>
+      </c>
+      <c r="B229">
+        <f>MEDIAN(B156:B226)</f>
+        <v>1</v>
+      </c>
+      <c r="F229">
+        <f t="shared" ref="C229:H229" si="8">MEDIAN(F156:F226)</f>
+        <v>81</v>
+      </c>
+      <c r="G229">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="H229">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>